<commit_message>
chore: (WIP) beautify write to file
</commit_message>
<xml_diff>
--- a/files/template_format_solution.xlsx
+++ b/files/template_format_solution.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9768"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Template Format Utama" sheetId="1" r:id="rId1"/>
@@ -1162,9 +1162,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:X1048559"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W4" sqref="W4:W6"/>
+      <selection pane="bottomLeft" activeCell="V72" sqref="V72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,7 +1191,7 @@
     <col min="20" max="20" width="18.33203125" style="17" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="41.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.44140625" style="1" customWidth="1"/>
     <col min="24" max="24" width="6.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="16384" width="8.88671875" style="1"/>
   </cols>

</xml_diff>